<commit_message>
created Sample_Test_Suite with all failed Testcases
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_SampleType-PrimMaligTumTissue.xlsx
+++ b/InputFiles/TC01_Canine_Filter_SampleType-PrimMaligTumTissue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF3ED24-A0E4-46BB-B68A-A15F4C86D9EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E507B7C4-6DF6-4DC6-98FC-1EB02DD77394}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -80,22 +80,6 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
-    <t>MATCH (s:study)
-  WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies
-  MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies
-  MATCH (d:diagnosis)
-  WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies
-  MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-  MATCH (samp:sample)-[*]-&gt;(c)
-  MATCH (f:file)-[*]-&gt;(c)
-  WHERE samp.summarized_sample_type IN ["Primary Malignant Tumor Tissue"]  
-  WITH DISTINCT c AS c, p, s, demo, diag, f, samp
-  RETURN count(DISTINCT(f)) as number_of_files ,
-             count(DISTINCT(samp)) as number_of_sample ,
-             count(DISTINCT(c.case_id)) as number_of_cases ,
-             count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
-  </si>
-  <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
@@ -130,6 +114,54 @@
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
         coalesce(diag.best_response, '') AS `Response to Treatment`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MATCH (p:program)&lt;--(s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+      WHERE (size([]) = 0 OR s.clinical_study_designation IN [])
+        AND (s.study_disposition = 'Unrestricted')
+        AND (size([]) = 0 OR s.clinical_study_type IN [])
+        AND (size(['Primary Malignant Tumor Tissue']) = 0 OR demo.breed IN ['Primary Malignant Tumor Tissue'])
+        AND (size([]) = 0 OR demo.sex IN [])
+        AND (size([]) = 0 OR demo.neutered_indicator IN [])
+        AND (size([]) = 0 OR diag.disease_term IN [])
+        AND (size([]) = 0 OR diag.primary_disease_site IN [])
+        AND (size([]) = 0 OR diag.stage_of_disease IN [])
+        AND (size([]) = 0 OR diag.best_response IN [])
+    OPTIONAL MATCH (c)--&gt;(co:cohort)
+    OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+    OPTIONAL MATCH (f)--&gt;(parent)
+    OPTIONAL MATCH (samp:sample)--&gt;(c)
+    OPTIONAL MATCH (samp)&lt;--(al:aliquot)
+    WITH DISTINCT c AS c, p, s, co, demo, diag, f, parent, samp, al
+      WHERE (size([]) = 0 OR samp.summarized_sample_type IN [])
+        AND (size([]) = 0 OR samp.specific_sample_pathology IN [])
+        AND (size([]) = 0 OR samp.sample_site IN [])
+        AND (size([]) = 0 OR head(labels(parent)) IN [])
+        AND (size([]) = 0 OR f.file_type IN [])
+        AND (size([]) = 0 OR f.file_format IN [])
+    WITH c.case_id AS case_id,
+         s.clinical_study_designation AS study_code,
+         s.clinical_study_type AS study_type,
+         co.cohort_description AS cohort,
+         demo.breed AS breed,
+         diag.disease_term AS diagnosis,
+         diag.stage_of_disease AS stage_of_disease,
+         diag.primary_disease_site AS disease_site,
+         demo.patient_age_at_enrollment AS age,
+         demo.sex AS sex,
+         demo.neutered_indicator AS neutered_status,
+         demo.weight AS weight,
+         diag.best_response AS response_to_treatment,
+         samp.sample_id AS sample_id,
+         f.uuid AS file_id,
+         al
+    RETURN
+COUNT(DISTINCT file_id) as number_of_files,
+COUNT(DISTINCT sample_id) as number_of_sample,
+COUNT(DISTINCT case_id) as number_of_cases,
+COUNT(DISTINCT study_code) as number_of_study,
+COUNT(DISTINCT al) as number_of_aliquot
+    </t>
   </si>
 </sst>
 </file>
@@ -501,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,15 +563,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -548,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -556,7 +588,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -565,15 +597,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fixed TC03,02,08,01,11,09,08 and Others
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_SampleType-PrimMaligTumTissue.xlsx
+++ b/InputFiles/TC01_Canine_Filter_SampleType-PrimMaligTumTissue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E507B7C4-6DF6-4DC6-98FC-1EB02DD77394}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6974BAE7-830B-4D20-95B8-7365B064758F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -120,7 +120,7 @@
       WHERE (size([]) = 0 OR s.clinical_study_designation IN [])
         AND (s.study_disposition = 'Unrestricted')
         AND (size([]) = 0 OR s.clinical_study_type IN [])
-        AND (size(['Primary Malignant Tumor Tissue']) = 0 OR demo.breed IN ['Primary Malignant Tumor Tissue'])
+        AND (size([]) = 0 OR demo.breed IN [])
         AND (size([]) = 0 OR demo.sex IN [])
         AND (size([]) = 0 OR demo.neutered_indicator IN [])
         AND (size([]) = 0 OR diag.disease_term IN [])
@@ -133,7 +133,7 @@
     OPTIONAL MATCH (samp:sample)--&gt;(c)
     OPTIONAL MATCH (samp)&lt;--(al:aliquot)
     WITH DISTINCT c AS c, p, s, co, demo, diag, f, parent, samp, al
-      WHERE (size([]) = 0 OR samp.summarized_sample_type IN [])
+      WHERE (size(['Primary Malignant Tumor Tissue']) = 0 OR samp.summarized_sample_type IN ['Primary Malignant Tumor Tissue'])
         AND (size([]) = 0 OR samp.specific_sample_pathology IN [])
         AND (size([]) = 0 OR samp.sample_site IN [])
         AND (size([]) = 0 OR head(labels(parent)) IN [])
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>